<commit_message>
Added restuls for Test Plan executoin (20 Sep)
</commit_message>
<xml_diff>
--- a/src/ssw567/assignment2/Test Plan.xlsx
+++ b/src/ssw567/assignment2/Test Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="222" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="222" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>SSW-567-WS Assignment 2 Test Plan</t>
   </si>
@@ -38,6 +38,9 @@
     <t>Pass or Fail</t>
   </si>
   <si>
+    <t>Note:</t>
+  </si>
+  <si>
     <t>1-1</t>
   </si>
   <si>
@@ -50,6 +53,12 @@
     <t>Program output "scalene"</t>
   </si>
   <si>
+    <t>Triangle is Scalene.</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
     <t>1-2</t>
   </si>
   <si>
@@ -59,19 +68,31 @@
     <t>Small number (isosceles triangle)</t>
   </si>
   <si>
-    <t>Program output "isosceles"</t>
+    <t>Invalid input.</t>
+  </si>
+  <si>
+    <t>Invalid input. Should be 3 integers.</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Our program currently only allows integers.</t>
   </si>
   <si>
     <t>1-3</t>
   </si>
   <si>
-    <t>Input         side1=1  side2=2      side1 =50         </t>
+    <t>Input         side1=1  side2=2      side3 =50</t>
   </si>
   <si>
     <t>Not a triangle</t>
   </si>
   <si>
     <t>Program catch the illegal input and output proper “Not triangle”</t>
+  </si>
+  <si>
+    <t>The 3 integers can't compose a triangle.</t>
   </si>
   <si>
     <t>2-1</t>
@@ -189,6 +210,9 @@
     <t>Valid Scalene/Right triangle</t>
   </si>
   <si>
+    <t>Triangle is Scalene. Triangle is Right.</t>
+  </si>
+  <si>
     <t>5-2</t>
   </si>
   <si>
@@ -199,6 +223,9 @@
   </si>
   <si>
     <t>Valid Isosceles/Equilateral triangle</t>
+  </si>
+  <si>
+    <t>Triangle is Equilateral. Triangle is Isosceles.</t>
   </si>
   <si>
     <t>5-3</t>
@@ -254,13 +281,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -276,12 +304,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -312,14 +334,14 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
       <right style="thin"/>
       <top style="thin"/>
@@ -328,67 +350,79 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+  <cellXfs count="10">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -458,349 +492,437 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="E5" activeCellId="0" pane="topLeft" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.9183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="18.9897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.7448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="28.4030612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="29.484693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.85" outlineLevel="0" r="3">
-      <c r="A3" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="88.7" outlineLevel="0" r="5">
-      <c r="A5" s="5" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="H4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.25" outlineLevel="0" r="6">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="F5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63.8" outlineLevel="0" r="7">
-      <c r="A7" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="38.95" outlineLevel="0" r="8">
-      <c r="A8" s="6" t="s">
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.4" outlineLevel="0" r="9">
-      <c r="A9" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.4" outlineLevel="0" r="10">
-      <c r="A10" s="6" t="s">
+      <c r="E7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="F7" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="38.95" outlineLevel="0" r="11">
-      <c r="A11" s="6" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63.8" outlineLevel="0" r="12">
-      <c r="A12" s="6" t="s">
+      <c r="E9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="38.95" outlineLevel="0" r="13">
-      <c r="A13" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.4" outlineLevel="0" r="14">
-      <c r="A14" s="6" t="s">
+      <c r="E11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.25" outlineLevel="0" r="15">
-      <c r="A15" s="6" t="s">
+      <c r="E12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="88.7" outlineLevel="0" r="16">
-      <c r="A16" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.4" outlineLevel="0" r="17">
-      <c r="A17" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="76.25" outlineLevel="0" r="18">
-      <c r="A18" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63.8" outlineLevel="0" r="19">
-      <c r="A19" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="63.8" outlineLevel="0" r="20">
-      <c r="A20" s="5" t="s">
+      <c r="F17" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="71.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.4" outlineLevel="0" r="21">
-      <c r="A21" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="F18" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.4" outlineLevel="0" r="22">
-      <c r="A22" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="E19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -812,9 +934,117 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
   </mergeCells>
+  <conditionalFormatting sqref="F11:F15,F5:F9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F19">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC33"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF0000FF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>